<commit_message>
Adding some missing files
</commit_message>
<xml_diff>
--- a/groundwork/rozbiti-kriterii.xlsx
+++ b/groundwork/rozbiti-kriterii.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="14620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="5240" yWindow="1900" windowWidth="25520" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="prvni hod" sheetId="2" r:id="rId1"/>
@@ -555,8 +555,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109228616"/>
-        <c:axId val="2109231608"/>
+        <c:axId val="2074980856"/>
+        <c:axId val="2074983848"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -619,11 +619,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109228616"/>
-        <c:axId val="2109231608"/>
+        <c:axId val="2074980856"/>
+        <c:axId val="2074983848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109228616"/>
+        <c:axId val="2074980856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109231608"/>
+        <c:crossAx val="2074983848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -640,7 +640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109231608"/>
+        <c:axId val="2074983848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,7 +651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109228616"/>
+        <c:crossAx val="2074980856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -662,6 +662,7 @@
         <c:idx val="2"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -952,8 +953,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109315464"/>
-        <c:axId val="2109318488"/>
+        <c:axId val="2075703048"/>
+        <c:axId val="2075706072"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1016,11 +1017,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109315464"/>
-        <c:axId val="2109318488"/>
+        <c:axId val="2075703048"/>
+        <c:axId val="2075706072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109315464"/>
+        <c:axId val="2075703048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,7 +1030,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109318488"/>
+        <c:crossAx val="2075706072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1037,7 +1038,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109318488"/>
+        <c:axId val="2075706072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1048,7 +1049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109315464"/>
+        <c:crossAx val="2075703048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1350,8 +1351,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109367512"/>
-        <c:axId val="2109370536"/>
+        <c:axId val="2075756344"/>
+        <c:axId val="2075759368"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1364,16 +1365,17 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
@@ -1414,11 +1416,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109367512"/>
-        <c:axId val="2109370536"/>
+        <c:axId val="2075756344"/>
+        <c:axId val="2075759368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109367512"/>
+        <c:axId val="2075756344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1427,7 +1429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109370536"/>
+        <c:crossAx val="2075759368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1435,7 +1437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109370536"/>
+        <c:axId val="2075759368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +1448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109367512"/>
+        <c:crossAx val="2075756344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1748,8 +1750,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109418872"/>
-        <c:axId val="2109421896"/>
+        <c:axId val="2075808968"/>
+        <c:axId val="2075811992"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1812,11 +1814,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109418872"/>
-        <c:axId val="2109421896"/>
+        <c:axId val="2075808968"/>
+        <c:axId val="2075811992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109418872"/>
+        <c:axId val="2075808968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1825,7 +1827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109421896"/>
+        <c:crossAx val="2075811992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1833,7 +1835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109421896"/>
+        <c:axId val="2075811992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,7 +1846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109418872"/>
+        <c:crossAx val="2075808968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2340,7 +2342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G138"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
       <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
@@ -7007,8 +7009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10604,7 +10606,7 @@
   <dimension ref="A1:I400"/>
   <sheetViews>
     <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="J133" sqref="J133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>